<commit_message>
updated the changes for the pr 7489
Signed-off-by: dishanktiwari2501 <dtiwari@progress.com>
</commit_message>
<xml_diff>
--- a/_vendor/github.com/chef/automate/components/docs-chef-io/static/calculator/automate_ha_hardware_calculator.xlsx
+++ b/_vendor/github.com/chef/automate/components/docs-chef-io/static/calculator/automate_ha_hardware_calculator.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7ED5448-1B21-445C-949E-1E2FAB459827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viyadav/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5232E58C-B100-5744-B8F9-C78375897D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="33320" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -248,7 +253,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,7 +425,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
@@ -440,6 +445,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -467,7 +476,6 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent6" xfId="1" builtinId="51"/>
@@ -885,31 +893,31 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="43.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" customWidth="1"/>
-    <col min="16" max="16" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20.1640625" customWidth="1"/>
+    <col min="12" max="12" width="10.5" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5" customWidth="1"/>
+    <col min="16" max="16" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="23.25">
+    <row r="1" spans="1:16" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75">
+    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -919,14 +927,14 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="21"/>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="23"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
@@ -934,7 +942,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="21">
+    <row r="4" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
@@ -944,20 +952,20 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="24"/>
-      <c r="L4" s="25" t="s">
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="26"/>
+      <c r="L4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="27"/>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="29"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
@@ -968,8 +976,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="18.75">
-      <c r="B6" s="28" t="s">
+    <row r="6" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="12">
@@ -997,7 +1005,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="18.75">
+    <row r="7" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>18</v>
       </c>
@@ -1015,11 +1023,11 @@
         <v>2</v>
       </c>
       <c r="M7" s="15">
-        <f ca="1">$C$34</f>
+        <f>$C$34</f>
         <v>2</v>
       </c>
       <c r="N7" s="15">
-        <f ca="1">INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$7,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
+        <f>INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$7,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
         <v>8</v>
       </c>
       <c r="O7" s="15" t="str">
@@ -1027,11 +1035,11 @@
         <v>80 GB</v>
       </c>
       <c r="P7" s="15" t="str">
-        <f ca="1">$C$35</f>
+        <f>$C$35</f>
         <v>m5.large</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="18.75">
+    <row r="8" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
       <c r="K8" s="15" t="s">
         <v>21</v>
@@ -1041,11 +1049,11 @@
         <v>2</v>
       </c>
       <c r="M8" s="15">
-        <f ca="1">$C$34</f>
+        <f>$C$34</f>
         <v>2</v>
       </c>
       <c r="N8" s="15">
-        <f ca="1">INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$8,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
+        <f>INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$8,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
         <v>8</v>
       </c>
       <c r="O8" s="15" t="str">
@@ -1053,11 +1061,11 @@
         <v>80 GB</v>
       </c>
       <c r="P8" s="15" t="str">
-        <f ca="1">$C$35</f>
+        <f>$C$35</f>
         <v>m5.large</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="18.75">
+    <row r="9" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>22</v>
       </c>
@@ -1074,11 +1082,11 @@
         <v>3</v>
       </c>
       <c r="M9" s="15">
-        <f ca="1">$C$34</f>
+        <f>$C$34</f>
         <v>2</v>
       </c>
       <c r="N9" s="16">
-        <f ca="1">INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$9,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
+        <f>INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$9,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
         <v>8</v>
       </c>
       <c r="O9" s="15" t="str">
@@ -1086,11 +1094,11 @@
         <v>150 GB</v>
       </c>
       <c r="P9" s="16" t="str">
-        <f ca="1">$C$35</f>
+        <f>$C$35</f>
         <v>m5.large</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="18.75">
+    <row r="10" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>25</v>
       </c>
@@ -1108,11 +1116,11 @@
         <v>3</v>
       </c>
       <c r="M10" s="15">
-        <f ca="1">INDEX(Sheet2!$C$2:'Sheet2'!$C$9,MATCH($P$10,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
+        <f>INDEX(Sheet2!$C$2:'Sheet2'!$C$9,MATCH($P$10,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
         <v>2</v>
       </c>
       <c r="N10" s="15">
-        <f ca="1">INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$10,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
+        <f>INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$10,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
         <v>8</v>
       </c>
       <c r="O10" s="15" t="str">
@@ -1120,12 +1128,12 @@
         <v>58.9 GB</v>
       </c>
       <c r="P10" s="15" t="str">
-        <f ca="1">$C$29</f>
+        <f>$C$29</f>
         <v>m5.large</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="18.75">
-      <c r="B11" s="28" t="s">
+    <row r="11" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="B11" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="17">
@@ -1141,11 +1149,11 @@
         <v>1</v>
       </c>
       <c r="M11" s="15">
-        <f ca="1">INDEX(Sheet2!$C$2:'Sheet2'!$C$9,MATCH($P$11,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
+        <f>INDEX(Sheet2!$C$2:'Sheet2'!$C$9,MATCH($P$11,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
         <v>2</v>
       </c>
       <c r="N11" s="15">
-        <f ca="1">INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$11,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
+        <f>INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$11,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
         <v>8</v>
       </c>
       <c r="O11" s="15" t="str">
@@ -1157,7 +1165,7 @@
         <v>m5.large</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
         <v>29</v>
       </c>
@@ -1165,54 +1173,55 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="L14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
-      <c r="B15" t="str">
-        <f xml:space="preserve"> _xlfn.CONCAT("All Scans should be run staggered i.e. spread out in a period of ",IF($D$5="Per Hour",60/$C$5,24/$C$5), IF($D$5="Per Hour"," minutes", " hours"))</f>
-        <v>All Scans should be run staggered i.e. spread out in a period of 60 minutes</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+    <row r="15" spans="1:16" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="20" t="str">
+        <f>IF($C$5=0,"",_xlfn.CONCAT("Client Runs should be run staggered i.e. spread out in a period of ",IF($D$5="Per Hour",60/$C$5,24/$C$5), IF($D$5="Per Hour"," minutes", " hours"))) &amp; CHAR(10) &amp; IF($C$4=0,"",_xlfn.CONCAT("Compliance Scans should be run staggered i.e. spread out in a period of ",IF($D$4="Per Hour",60/$C$4,24/$C$4), IF($D$4="Per Hour"," minutes", " hours")))</f>
+        <v>Client Runs should be run staggered i.e. spread out in a period of 60 minutes
+Compliance Scans should be run staggered i.e. spread out in a period of 60 minutes</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="1">
-        <f>$C$3/IF($D$4="Per Hour",(60/$C$4)*0.5,(24/$C$4)*60*0.5)</f>
+        <f>IF($C$4=0,0,$C$3/IF($D$4="Per Hour",(60/$C$4)*0.5,(24/$C$4)*60*0.5))</f>
         <v>166.66666666666666</v>
       </c>
       <c r="D16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="2">
-        <f>$C$3/IF($D$5="Per Hour",(60/$C$5)*0.5,(24/$C$5)*60*0.5)</f>
+        <f>IF($C$5=0,0,$C$3/IF($D$5="Per Hour",(60/$C$5)*0.5,(24/$C$5)*60*0.5))</f>
         <v>166.66666666666666</v>
       </c>
       <c r="D17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="1">
-        <f>$C$3/IF($D$6="Per Hour",(60/$C$6)*0.5,(24/$C$6)*60*0.5)</f>
+        <f>IF($C$6=0,0,$C$3/IF($D$6="Per Hour",(60/$C$6)*0.5,(24/$C$6)*60*0.5))</f>
         <v>166.66666666666666</v>
       </c>
       <c r="D18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>35</v>
       </c>
@@ -1224,7 +1233,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>37</v>
       </c>
@@ -1236,7 +1245,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>38</v>
       </c>
@@ -1248,7 +1257,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>39</v>
       </c>
@@ -1256,12 +1265,12 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="21">
+    <row r="25" spans="2:4" ht="21" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
         <v>41</v>
       </c>
@@ -1271,7 +1280,7 @@
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>42</v>
       </c>
@@ -1283,24 +1292,24 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C28" s="5" cm="1">
-        <f t="array" aca="1" ref="C28" ca="1">INDEX(Sheet2!A2:'Sheet2'!A9,MATCH(MIN(ABS(Sheet2!A2:'Sheet2'!A9-$C$27)),ABS(Sheet2!A2:'Sheet2'!A9-$C$27),0))</f>
+        <f t="array" ref="C28">INDEX(Sheet2!A2:'Sheet2'!A9,MATCH(MIN(ABS(Sheet2!A2:'Sheet2'!A9-$C$27)),ABS(Sheet2!A2:'Sheet2'!A9-$C$27),0))</f>
         <v>8</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="C29" ca="1">INDEX(Sheet2!$B$2:'Sheet2'!$B$9,MATCH(MIN(ABS(Sheet2!$A$2:'Sheet2'!$A$9-$C$27)),ABS(Sheet2!$A$2:'Sheet2'!$A$9-$C$27),0))</f>
+        <f t="array" ref="C29">INDEX(Sheet2!$B$2:'Sheet2'!$B$9,MATCH(MIN(ABS(Sheet2!$A$2:'Sheet2'!$A$9-$C$27)),ABS(Sheet2!$A$2:'Sheet2'!$A$9-$C$27),0))</f>
         <v>m5.large</v>
       </c>
       <c r="D29" s="5" t="str">
@@ -1308,7 +1317,7 @@
         <v xml:space="preserve">   3 number of nodes</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
         <v>46</v>
       </c>
@@ -1317,7 +1326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:7">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>47</v>
       </c>
@@ -1329,24 +1338,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="2:7">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C34" s="5" cm="1">
-        <f t="array" aca="1" ref="C34" ca="1">INDEX(Sheet2!C2:'Sheet2'!C9,MATCH(MIN(ABS(Sheet2!C2:'Sheet2'!C9-$C$33)),ABS(Sheet2!C2:'Sheet2'!C9-$C$33),0))</f>
+        <f t="array" ref="C34">INDEX(Sheet2!C2:'Sheet2'!C9,MATCH(MIN(ABS(Sheet2!C2:'Sheet2'!C9-$C$33)),ABS(Sheet2!C2:'Sheet2'!C9-$C$33),0))</f>
         <v>2</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="2:7">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C35" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="C35" ca="1">INDEX(Sheet2!$B$2:'Sheet2'!$B$9,MATCH(MIN(ABS(Sheet2!$C$2:'Sheet2'!$C$9-$C$33)),ABS(Sheet2!$C$2:'Sheet2'!$C$9-$C$33),0))</f>
+        <f t="array" ref="C35">INDEX(Sheet2!$B$2:'Sheet2'!$B$9,MATCH(MIN(ABS(Sheet2!$C$2:'Sheet2'!$C$9-$C$33)),ABS(Sheet2!$C$2:'Sheet2'!$C$9-$C$33),0))</f>
         <v>m5.large</v>
       </c>
       <c r="D35" s="5" t="str">
@@ -1354,7 +1363,7 @@
         <v xml:space="preserve">   2 number of nodes</v>
       </c>
     </row>
-    <row r="38" spans="2:7">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>50</v>
       </c>
@@ -1368,7 +1377,7 @@
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
     </row>
-    <row r="39" spans="2:7">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
         <v>51</v>
       </c>
@@ -1391,7 +1400,7 @@
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="L4:O4"/>
   </mergeCells>
-  <dataValidations count="12">
+  <dataValidations count="13">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D9:D11" xr:uid="{3F9CC802-860F-476F-9E8C-ABA15EB1CF86}">
       <formula1>"MB, KB"</formula1>
     </dataValidation>
@@ -1421,7 +1430,7 @@
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10 C4:C5" xr:uid="{EA4BC509-8784-4E6C-8111-83A3B4B8C7D4}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10" xr:uid="{EA4BC509-8784-4E6C-8111-83A3B4B8C7D4}">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -1434,6 +1443,10 @@
     <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{BB28DE5A-016B-412A-81CF-C2EEF0876B85}">
       <formula1>0.0001</formula1>
       <formula2>1024</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4 C5 C6" xr:uid="{D028250A-DA0C-DF4B-A681-2950108A8ED1}">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1452,9 +1465,9 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1465,7 +1478,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>8</v>
       </c>
@@ -1476,7 +1489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>16</v>
       </c>
@@ -1487,7 +1500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>32</v>
       </c>
@@ -1498,7 +1511,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>64</v>
       </c>
@@ -1509,7 +1522,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>128</v>
       </c>
@@ -1520,7 +1533,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>192</v>
       </c>
@@ -1531,7 +1544,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>256</v>
       </c>
@@ -1542,7 +1555,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>384</v>
       </c>
@@ -1560,6 +1573,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5712601c-4137-4c53-ac8c-2395ac8d0b4e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <ebco xmlns="5712601c-4137-4c53-ac8c-2395ac8d0b4e" xsi:nil="true"/>
+    <TaxCatchAll xmlns="0dfb052e-cb13-4d19-82cf-940ca1bb85b7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AF27FAE51E038C41BAD01F89945E9328" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="794a841236f158cc08bab6d8dae19bba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5712601c-4137-4c53-ac8c-2395ac8d0b4e" xmlns:ns3="77bfaf30-28d1-46cd-bb4b-b6e7f7a97e42" xmlns:ns4="0dfb052e-cb13-4d19-82cf-940ca1bb85b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cd6e02a022e236667f2c94c6418cf3af" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="5712601c-4137-4c53-ac8c-2395ac8d0b4e"/>
@@ -1813,18 +1838,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5712601c-4137-4c53-ac8c-2395ac8d0b4e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <ebco xmlns="5712601c-4137-4c53-ac8c-2395ac8d0b4e" xsi:nil="true"/>
-    <TaxCatchAll xmlns="0dfb052e-cb13-4d19-82cf-940ca1bb85b7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1835,13 +1848,40 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2DCFC80-DE31-4D62-BE6F-AEE54BCB3A5D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23643DB7-AF00-4C10-B696-5877E2243C0A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5712601c-4137-4c53-ac8c-2395ac8d0b4e"/>
+    <ds:schemaRef ds:uri="0dfb052e-cb13-4d19-82cf-940ca1bb85b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23643DB7-AF00-4C10-B696-5877E2243C0A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2DCFC80-DE31-4D62-BE6F-AEE54BCB3A5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5712601c-4137-4c53-ac8c-2395ac8d0b4e"/>
+    <ds:schemaRef ds:uri="77bfaf30-28d1-46cd-bb4b-b6e7f7a97e42"/>
+    <ds:schemaRef ds:uri="0dfb052e-cb13-4d19-82cf-940ca1bb85b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14702B79-0641-4C37-B714-6CDAE45636B7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14702B79-0641-4C37-B714-6CDAE45636B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated the changes for the pr 7489 (#3988)
Signed-off-by: dishanktiwari2501 <dtiwari@progress.com>

Signed-off-by: dishanktiwari2501 <dtiwari@progress.com>
</commit_message>
<xml_diff>
--- a/_vendor/github.com/chef/automate/components/docs-chef-io/static/calculator/automate_ha_hardware_calculator.xlsx
+++ b/_vendor/github.com/chef/automate/components/docs-chef-io/static/calculator/automate_ha_hardware_calculator.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7ED5448-1B21-445C-949E-1E2FAB459827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viyadav/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5232E58C-B100-5744-B8F9-C78375897D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="33320" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -248,7 +253,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,7 +425,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
@@ -440,6 +445,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -467,7 +476,6 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent6" xfId="1" builtinId="51"/>
@@ -885,31 +893,31 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="43.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" customWidth="1"/>
-    <col min="16" max="16" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20.1640625" customWidth="1"/>
+    <col min="12" max="12" width="10.5" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5" customWidth="1"/>
+    <col min="16" max="16" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="23.25">
+    <row r="1" spans="1:16" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75">
+    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -919,14 +927,14 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="21"/>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="23"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
@@ -934,7 +942,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="21">
+    <row r="4" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
@@ -944,20 +952,20 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="24"/>
-      <c r="L4" s="25" t="s">
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="26"/>
+      <c r="L4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="27"/>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="29"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
@@ -968,8 +976,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="18.75">
-      <c r="B6" s="28" t="s">
+    <row r="6" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="12">
@@ -997,7 +1005,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="18.75">
+    <row r="7" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>18</v>
       </c>
@@ -1015,11 +1023,11 @@
         <v>2</v>
       </c>
       <c r="M7" s="15">
-        <f ca="1">$C$34</f>
+        <f>$C$34</f>
         <v>2</v>
       </c>
       <c r="N7" s="15">
-        <f ca="1">INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$7,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
+        <f>INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$7,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
         <v>8</v>
       </c>
       <c r="O7" s="15" t="str">
@@ -1027,11 +1035,11 @@
         <v>80 GB</v>
       </c>
       <c r="P7" s="15" t="str">
-        <f ca="1">$C$35</f>
+        <f>$C$35</f>
         <v>m5.large</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="18.75">
+    <row r="8" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
       <c r="K8" s="15" t="s">
         <v>21</v>
@@ -1041,11 +1049,11 @@
         <v>2</v>
       </c>
       <c r="M8" s="15">
-        <f ca="1">$C$34</f>
+        <f>$C$34</f>
         <v>2</v>
       </c>
       <c r="N8" s="15">
-        <f ca="1">INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$8,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
+        <f>INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$8,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
         <v>8</v>
       </c>
       <c r="O8" s="15" t="str">
@@ -1053,11 +1061,11 @@
         <v>80 GB</v>
       </c>
       <c r="P8" s="15" t="str">
-        <f ca="1">$C$35</f>
+        <f>$C$35</f>
         <v>m5.large</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="18.75">
+    <row r="9" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>22</v>
       </c>
@@ -1074,11 +1082,11 @@
         <v>3</v>
       </c>
       <c r="M9" s="15">
-        <f ca="1">$C$34</f>
+        <f>$C$34</f>
         <v>2</v>
       </c>
       <c r="N9" s="16">
-        <f ca="1">INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$9,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
+        <f>INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$9,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
         <v>8</v>
       </c>
       <c r="O9" s="15" t="str">
@@ -1086,11 +1094,11 @@
         <v>150 GB</v>
       </c>
       <c r="P9" s="16" t="str">
-        <f ca="1">$C$35</f>
+        <f>$C$35</f>
         <v>m5.large</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="18.75">
+    <row r="10" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>25</v>
       </c>
@@ -1108,11 +1116,11 @@
         <v>3</v>
       </c>
       <c r="M10" s="15">
-        <f ca="1">INDEX(Sheet2!$C$2:'Sheet2'!$C$9,MATCH($P$10,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
+        <f>INDEX(Sheet2!$C$2:'Sheet2'!$C$9,MATCH($P$10,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
         <v>2</v>
       </c>
       <c r="N10" s="15">
-        <f ca="1">INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$10,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
+        <f>INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$10,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
         <v>8</v>
       </c>
       <c r="O10" s="15" t="str">
@@ -1120,12 +1128,12 @@
         <v>58.9 GB</v>
       </c>
       <c r="P10" s="15" t="str">
-        <f ca="1">$C$29</f>
+        <f>$C$29</f>
         <v>m5.large</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="18.75">
-      <c r="B11" s="28" t="s">
+    <row r="11" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="B11" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="17">
@@ -1141,11 +1149,11 @@
         <v>1</v>
       </c>
       <c r="M11" s="15">
-        <f ca="1">INDEX(Sheet2!$C$2:'Sheet2'!$C$9,MATCH($P$11,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
+        <f>INDEX(Sheet2!$C$2:'Sheet2'!$C$9,MATCH($P$11,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
         <v>2</v>
       </c>
       <c r="N11" s="15">
-        <f ca="1">INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$11,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
+        <f>INDEX(Sheet2!$A$2:'Sheet2'!$A$9,MATCH($P$11,Sheet2!$B$2:'Sheet2'!$B$9,0))</f>
         <v>8</v>
       </c>
       <c r="O11" s="15" t="str">
@@ -1157,7 +1165,7 @@
         <v>m5.large</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
         <v>29</v>
       </c>
@@ -1165,54 +1173,55 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="L14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
-      <c r="B15" t="str">
-        <f xml:space="preserve"> _xlfn.CONCAT("All Scans should be run staggered i.e. spread out in a period of ",IF($D$5="Per Hour",60/$C$5,24/$C$5), IF($D$5="Per Hour"," minutes", " hours"))</f>
-        <v>All Scans should be run staggered i.e. spread out in a period of 60 minutes</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+    <row r="15" spans="1:16" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="20" t="str">
+        <f>IF($C$5=0,"",_xlfn.CONCAT("Client Runs should be run staggered i.e. spread out in a period of ",IF($D$5="Per Hour",60/$C$5,24/$C$5), IF($D$5="Per Hour"," minutes", " hours"))) &amp; CHAR(10) &amp; IF($C$4=0,"",_xlfn.CONCAT("Compliance Scans should be run staggered i.e. spread out in a period of ",IF($D$4="Per Hour",60/$C$4,24/$C$4), IF($D$4="Per Hour"," minutes", " hours")))</f>
+        <v>Client Runs should be run staggered i.e. spread out in a period of 60 minutes
+Compliance Scans should be run staggered i.e. spread out in a period of 60 minutes</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="1">
-        <f>$C$3/IF($D$4="Per Hour",(60/$C$4)*0.5,(24/$C$4)*60*0.5)</f>
+        <f>IF($C$4=0,0,$C$3/IF($D$4="Per Hour",(60/$C$4)*0.5,(24/$C$4)*60*0.5))</f>
         <v>166.66666666666666</v>
       </c>
       <c r="D16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="2">
-        <f>$C$3/IF($D$5="Per Hour",(60/$C$5)*0.5,(24/$C$5)*60*0.5)</f>
+        <f>IF($C$5=0,0,$C$3/IF($D$5="Per Hour",(60/$C$5)*0.5,(24/$C$5)*60*0.5))</f>
         <v>166.66666666666666</v>
       </c>
       <c r="D17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="1">
-        <f>$C$3/IF($D$6="Per Hour",(60/$C$6)*0.5,(24/$C$6)*60*0.5)</f>
+        <f>IF($C$6=0,0,$C$3/IF($D$6="Per Hour",(60/$C$6)*0.5,(24/$C$6)*60*0.5))</f>
         <v>166.66666666666666</v>
       </c>
       <c r="D18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>35</v>
       </c>
@@ -1224,7 +1233,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>37</v>
       </c>
@@ -1236,7 +1245,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>38</v>
       </c>
@@ -1248,7 +1257,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>39</v>
       </c>
@@ -1256,12 +1265,12 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="21">
+    <row r="25" spans="2:4" ht="21" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
         <v>41</v>
       </c>
@@ -1271,7 +1280,7 @@
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>42</v>
       </c>
@@ -1283,24 +1292,24 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C28" s="5" cm="1">
-        <f t="array" aca="1" ref="C28" ca="1">INDEX(Sheet2!A2:'Sheet2'!A9,MATCH(MIN(ABS(Sheet2!A2:'Sheet2'!A9-$C$27)),ABS(Sheet2!A2:'Sheet2'!A9-$C$27),0))</f>
+        <f t="array" ref="C28">INDEX(Sheet2!A2:'Sheet2'!A9,MATCH(MIN(ABS(Sheet2!A2:'Sheet2'!A9-$C$27)),ABS(Sheet2!A2:'Sheet2'!A9-$C$27),0))</f>
         <v>8</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="C29" ca="1">INDEX(Sheet2!$B$2:'Sheet2'!$B$9,MATCH(MIN(ABS(Sheet2!$A$2:'Sheet2'!$A$9-$C$27)),ABS(Sheet2!$A$2:'Sheet2'!$A$9-$C$27),0))</f>
+        <f t="array" ref="C29">INDEX(Sheet2!$B$2:'Sheet2'!$B$9,MATCH(MIN(ABS(Sheet2!$A$2:'Sheet2'!$A$9-$C$27)),ABS(Sheet2!$A$2:'Sheet2'!$A$9-$C$27),0))</f>
         <v>m5.large</v>
       </c>
       <c r="D29" s="5" t="str">
@@ -1308,7 +1317,7 @@
         <v xml:space="preserve">   3 number of nodes</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
         <v>46</v>
       </c>
@@ -1317,7 +1326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:7">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>47</v>
       </c>
@@ -1329,24 +1338,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="2:7">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C34" s="5" cm="1">
-        <f t="array" aca="1" ref="C34" ca="1">INDEX(Sheet2!C2:'Sheet2'!C9,MATCH(MIN(ABS(Sheet2!C2:'Sheet2'!C9-$C$33)),ABS(Sheet2!C2:'Sheet2'!C9-$C$33),0))</f>
+        <f t="array" ref="C34">INDEX(Sheet2!C2:'Sheet2'!C9,MATCH(MIN(ABS(Sheet2!C2:'Sheet2'!C9-$C$33)),ABS(Sheet2!C2:'Sheet2'!C9-$C$33),0))</f>
         <v>2</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="2:7">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C35" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="C35" ca="1">INDEX(Sheet2!$B$2:'Sheet2'!$B$9,MATCH(MIN(ABS(Sheet2!$C$2:'Sheet2'!$C$9-$C$33)),ABS(Sheet2!$C$2:'Sheet2'!$C$9-$C$33),0))</f>
+        <f t="array" ref="C35">INDEX(Sheet2!$B$2:'Sheet2'!$B$9,MATCH(MIN(ABS(Sheet2!$C$2:'Sheet2'!$C$9-$C$33)),ABS(Sheet2!$C$2:'Sheet2'!$C$9-$C$33),0))</f>
         <v>m5.large</v>
       </c>
       <c r="D35" s="5" t="str">
@@ -1354,7 +1363,7 @@
         <v xml:space="preserve">   2 number of nodes</v>
       </c>
     </row>
-    <row r="38" spans="2:7">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>50</v>
       </c>
@@ -1368,7 +1377,7 @@
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
     </row>
-    <row r="39" spans="2:7">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
         <v>51</v>
       </c>
@@ -1391,7 +1400,7 @@
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="L4:O4"/>
   </mergeCells>
-  <dataValidations count="12">
+  <dataValidations count="13">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D9:D11" xr:uid="{3F9CC802-860F-476F-9E8C-ABA15EB1CF86}">
       <formula1>"MB, KB"</formula1>
     </dataValidation>
@@ -1421,7 +1430,7 @@
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10 C4:C5" xr:uid="{EA4BC509-8784-4E6C-8111-83A3B4B8C7D4}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10" xr:uid="{EA4BC509-8784-4E6C-8111-83A3B4B8C7D4}">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -1434,6 +1443,10 @@
     <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{BB28DE5A-016B-412A-81CF-C2EEF0876B85}">
       <formula1>0.0001</formula1>
       <formula2>1024</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4 C5 C6" xr:uid="{D028250A-DA0C-DF4B-A681-2950108A8ED1}">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1452,9 +1465,9 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1465,7 +1478,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>8</v>
       </c>
@@ -1476,7 +1489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>16</v>
       </c>
@@ -1487,7 +1500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>32</v>
       </c>
@@ -1498,7 +1511,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>64</v>
       </c>
@@ -1509,7 +1522,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>128</v>
       </c>
@@ -1520,7 +1533,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>192</v>
       </c>
@@ -1531,7 +1544,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>256</v>
       </c>
@@ -1542,7 +1555,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>384</v>
       </c>
@@ -1560,6 +1573,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5712601c-4137-4c53-ac8c-2395ac8d0b4e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <ebco xmlns="5712601c-4137-4c53-ac8c-2395ac8d0b4e" xsi:nil="true"/>
+    <TaxCatchAll xmlns="0dfb052e-cb13-4d19-82cf-940ca1bb85b7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AF27FAE51E038C41BAD01F89945E9328" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="794a841236f158cc08bab6d8dae19bba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5712601c-4137-4c53-ac8c-2395ac8d0b4e" xmlns:ns3="77bfaf30-28d1-46cd-bb4b-b6e7f7a97e42" xmlns:ns4="0dfb052e-cb13-4d19-82cf-940ca1bb85b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cd6e02a022e236667f2c94c6418cf3af" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="5712601c-4137-4c53-ac8c-2395ac8d0b4e"/>
@@ -1813,18 +1838,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5712601c-4137-4c53-ac8c-2395ac8d0b4e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <ebco xmlns="5712601c-4137-4c53-ac8c-2395ac8d0b4e" xsi:nil="true"/>
-    <TaxCatchAll xmlns="0dfb052e-cb13-4d19-82cf-940ca1bb85b7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1835,13 +1848,40 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2DCFC80-DE31-4D62-BE6F-AEE54BCB3A5D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23643DB7-AF00-4C10-B696-5877E2243C0A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5712601c-4137-4c53-ac8c-2395ac8d0b4e"/>
+    <ds:schemaRef ds:uri="0dfb052e-cb13-4d19-82cf-940ca1bb85b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23643DB7-AF00-4C10-B696-5877E2243C0A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2DCFC80-DE31-4D62-BE6F-AEE54BCB3A5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5712601c-4137-4c53-ac8c-2395ac8d0b4e"/>
+    <ds:schemaRef ds:uri="77bfaf30-28d1-46cd-bb4b-b6e7f7a97e42"/>
+    <ds:schemaRef ds:uri="0dfb052e-cb13-4d19-82cf-940ca1bb85b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14702B79-0641-4C37-B714-6CDAE45636B7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14702B79-0641-4C37-B714-6CDAE45636B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>